<commit_message>
correction lien vers profinfo
</commit_message>
<xml_diff>
--- a/template/horaire-rencontres.xlsx
+++ b/template/horaire-rencontres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/projetpersonnel/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7827A6DB-078D-B24C-8EE1-DBE2CC5F2931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDF3B78-91EA-7644-BDC1-18C2CF11C0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1580" windowWidth="27080" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B11" sqref="B11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,11 +528,11 @@
         <v>45875.541666666664</v>
       </c>
       <c r="B2" t="str">
-        <f>"1937092"</f>
-        <v>1937092</v>
+        <f>"2141316"</f>
+        <v>2141316</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -644,11 +644,11 @@
         <v>45875.635416666642</v>
       </c>
       <c r="B11" t="str">
-        <f>"2141316"</f>
-        <v>2141316</v>
+        <f>"1937092"</f>
+        <v>1937092</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>